<commit_message>
link to survey deleted
</commit_message>
<xml_diff>
--- a/emissions isolation.xlsx
+++ b/emissions isolation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra-my.sharepoint.com/personal/jpueyo_icra_cat/Documents/Edicitnet_JPR/tygron/excel_indicators/NO2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{81FF2161-9837-4B7C-A4C0-9BD898CE21C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B69444B-C8A9-48CC-90DC-DC14FF2DD0B8}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{81FF2161-9837-4B7C-A4C0-9BD898CE21C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F2C6319-C2BE-4A23-9B38-4A270ADE8E35}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{669AB16C-4124-4831-908F-D718A00C437F}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669AB16C-4124-4831-908F-D718A00C437F}"/>
   </bookViews>
   <sheets>
     <sheet name="intent_01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E738F8BE-7D0B-40E2-9227-CAEA18510AD0}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="D1">
-        <v>15</v>
+        <v>5.13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
       </c>
       <c r="D3" s="1">
         <f>D1-D2</f>
-        <v>15</v>
+        <v>5.13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -808,7 +808,7 @@
       </c>
       <c r="D9">
         <f>D4*D7+D5*D6-D3*(1-D4)</f>
-        <v>18.250000000000004</v>
+        <v>27.429100000000005</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
       </c>
       <c r="D10">
         <f>D3*(1-D4)</f>
-        <v>13.95</v>
+        <v>4.7708999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -838,7 +838,7 @@
       </c>
       <c r="D11">
         <f>(-D9+SQRT(D9^2+4*D8*D10))/2*D8</f>
-        <v>3.230680131588809E-3</v>
+        <v>7.3683722704277256E-4</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>3</v>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -902,7 +902,7 @@
       </c>
       <c r="D15" s="1">
         <f>D11/(D12*D13*D14)</f>
-        <v>6.3160901888344251E-2</v>
+        <v>4.001505523203934E-3</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -920,7 +920,7 @@
       </c>
       <c r="D16">
         <f>D15*D4</f>
-        <v>4.4212631321840978E-3</v>
+        <v>2.801053866242754E-4</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -938,7 +938,7 @@
       </c>
       <c r="D17">
         <f>D15+D16</f>
-        <v>6.7582165020528343E-2</v>
+        <v>4.2816109098282092E-3</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -955,7 +955,7 @@
         <v>38</v>
       </c>
       <c r="D18">
-        <v>18075</v>
+        <v>8003</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
@@ -973,7 +973,7 @@
       </c>
       <c r="D19" s="3">
         <f>D17*D18</f>
-        <v>1221.5476327460499</v>
+        <v>34.265732111355156</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
@@ -988,18 +988,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1226,18 +1226,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C3283C-ECF4-4D35-98F3-35B008220AF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AE9B3-AB7F-4964-AE03-9E5C0AEC7C40}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AE9B3-AB7F-4964-AE03-9E5C0AEC7C40}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C3283C-ECF4-4D35-98F3-35B008220AF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Revert "link to survey deleted"
This reverts commit f5314d316ae34e760ff931883c3d940bed9f7497.
</commit_message>
<xml_diff>
--- a/emissions isolation.xlsx
+++ b/emissions isolation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra-my.sharepoint.com/personal/jpueyo_icra_cat/Documents/Edicitnet_JPR/tygron/excel_indicators/NO2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{81FF2161-9837-4B7C-A4C0-9BD898CE21C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6F2C6319-C2BE-4A23-9B38-4A270ADE8E35}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{81FF2161-9837-4B7C-A4C0-9BD898CE21C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B69444B-C8A9-48CC-90DC-DC14FF2DD0B8}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{669AB16C-4124-4831-908F-D718A00C437F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{669AB16C-4124-4831-908F-D718A00C437F}"/>
   </bookViews>
   <sheets>
     <sheet name="intent_01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E738F8BE-7D0B-40E2-9227-CAEA18510AD0}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>25</v>
       </c>
       <c r="D1">
-        <v>5.13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
       </c>
       <c r="D3" s="1">
         <f>D1-D2</f>
-        <v>5.13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -808,7 +808,7 @@
       </c>
       <c r="D9">
         <f>D4*D7+D5*D6-D3*(1-D4)</f>
-        <v>27.429100000000005</v>
+        <v>18.250000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
       </c>
       <c r="D10">
         <f>D3*(1-D4)</f>
-        <v>4.7708999999999993</v>
+        <v>13.95</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -838,7 +838,7 @@
       </c>
       <c r="D11">
         <f>(-D9+SQRT(D9^2+4*D8*D10))/2*D8</f>
-        <v>7.3683722704277256E-4</v>
+        <v>3.230680131588809E-3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>3</v>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>1.8</v>
+        <v>0.5</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -902,7 +902,7 @@
       </c>
       <c r="D15" s="1">
         <f>D11/(D12*D13*D14)</f>
-        <v>4.001505523203934E-3</v>
+        <v>6.3160901888344251E-2</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -920,7 +920,7 @@
       </c>
       <c r="D16">
         <f>D15*D4</f>
-        <v>2.801053866242754E-4</v>
+        <v>4.4212631321840978E-3</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -938,7 +938,7 @@
       </c>
       <c r="D17">
         <f>D15+D16</f>
-        <v>4.2816109098282092E-3</v>
+        <v>6.7582165020528343E-2</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -955,7 +955,7 @@
         <v>38</v>
       </c>
       <c r="D18">
-        <v>8003</v>
+        <v>18075</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
@@ -973,7 +973,7 @@
       </c>
       <c r="D19" s="3">
         <f>D17*D18</f>
-        <v>34.265732111355156</v>
+        <v>1221.5476327460499</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
@@ -988,18 +988,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1226,18 +1226,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AE9B3-AB7F-4964-AE03-9E5C0AEC7C40}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C3283C-ECF4-4D35-98F3-35B008220AF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C3283C-ECF4-4D35-98F3-35B008220AF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AE9B3-AB7F-4964-AE03-9E5C0AEC7C40}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>